<commit_message>
metric01b supporting Excel file
cleaned up
</commit_message>
<xml_diff>
--- a/2025_update/census_bps_monthly_2015_Oct2025.xlsx
+++ b/2025_update/census_bps_monthly_2015_Oct2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\housing-permits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA81F5C6-1B20-4F4C-BAD1-C659F052036A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC559C88-FB5B-4264-AE65-AF08BFD6E2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="90">
   <si>
     <t>CSA</t>
   </si>
@@ -723,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q263"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
-      <selection activeCell="F262" sqref="F262"/>
+    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
+      <selection activeCell="A263" sqref="A263:XFD263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9956,55 +9956,23 @@
       <c r="P261" s="23"/>
     </row>
     <row r="263" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A263" s="24">
-        <v>500</v>
-      </c>
-      <c r="B263" s="24">
-        <v>42660</v>
-      </c>
-      <c r="C263" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D263" s="25">
-        <v>2</v>
-      </c>
-      <c r="E263" s="24">
-        <v>1192</v>
-      </c>
-      <c r="F263" s="24">
-        <v>441</v>
-      </c>
-      <c r="G263" s="24">
-        <v>68</v>
-      </c>
-      <c r="H263" s="25">
-        <v>69</v>
-      </c>
-      <c r="I263" s="25">
-        <v>614</v>
-      </c>
-      <c r="J263" s="25">
-        <v>29</v>
-      </c>
+      <c r="A263" s="24"/>
+      <c r="B263" s="24"/>
+      <c r="C263" s="24"/>
+      <c r="D263" s="25"/>
+      <c r="E263" s="24"/>
+      <c r="F263" s="24"/>
+      <c r="G263" s="24"/>
+      <c r="H263" s="25"/>
+      <c r="I263" s="25"/>
+      <c r="J263" s="25"/>
       <c r="K263" s="24"/>
-      <c r="L263" s="24">
-        <v>6493</v>
-      </c>
-      <c r="M263" s="24">
-        <v>3155</v>
-      </c>
-      <c r="N263" s="24">
-        <v>462</v>
-      </c>
-      <c r="O263" s="25">
-        <v>265</v>
-      </c>
-      <c r="P263" s="25">
-        <v>2611</v>
-      </c>
-      <c r="Q263" s="25">
-        <v>120</v>
-      </c>
+      <c r="L263" s="24"/>
+      <c r="M263" s="24"/>
+      <c r="N263" s="24"/>
+      <c r="O263" s="25"/>
+      <c r="P263" s="25"/>
+      <c r="Q263" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A98:K197">

</xml_diff>